<commit_message>
changes in the SR Details prompt
</commit_message>
<xml_diff>
--- a/SRDetails.xlsx
+++ b/SRDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monalisa\Documents\Git\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A639B789-9F9D-4B84-A921-115F05FB2C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0424B6DE-F434-46C1-A435-B821D69D5D3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>SRNumber</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">Work in progress. With technical team </t>
+  </si>
+  <si>
+    <t>ETA</t>
   </si>
 </sst>
 </file>
@@ -87,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,79 +373,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="1">
+        <v>44065</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="1">
+        <v>43885</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="1">
+        <v>43705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" s="1">
+        <v>43525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="1">
+        <v>43345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="1">
+        <v>43165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding proactive file, creds for http and incident description intent
</commit_message>
<xml_diff>
--- a/SRDetails.xlsx
+++ b/SRDetails.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monalisa\Documents\Git\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monalisa\Documents\Rasaproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C448823-E26B-4CD6-9E29-0A2480F78DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F6FD6E-C8E8-4A69-9A15-0D895B9AF822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>SRNumber</t>
   </si>
@@ -33,38 +33,47 @@
     <t>Update</t>
   </si>
   <si>
-    <t>SR12345RE</t>
-  </si>
-  <si>
-    <t>SR13465RE</t>
-  </si>
-  <si>
-    <t>SR13265RE</t>
-  </si>
-  <si>
-    <t>SR13468RE</t>
-  </si>
-  <si>
-    <t>SR13460RE</t>
-  </si>
-  <si>
-    <t>SR13225RE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Work in progress. With technical team </t>
   </si>
   <si>
     <t>ETA</t>
+  </si>
+  <si>
+    <t>SR1234567</t>
+  </si>
+  <si>
+    <t>SR2345678</t>
+  </si>
+  <si>
+    <t>SR3456789</t>
+  </si>
+  <si>
+    <t>SR4567900</t>
+  </si>
+  <si>
+    <t>SR5679011</t>
+  </si>
+  <si>
+    <t>SR6790122</t>
+  </si>
+  <si>
+    <t>SR7901233</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -393,15 +402,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
         <v>44065</v>
@@ -409,10 +418,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>43885</v>
@@ -420,10 +429,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>43705</v>
@@ -431,10 +440,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>43525</v>
@@ -442,10 +451,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>43345</v>
@@ -453,10 +462,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>43165</v>
@@ -464,16 +473,17 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <v>42985</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>